<commit_message>
fix: Mejorar parseo de fechas para soportar múltiples formatos
</commit_message>
<xml_diff>
--- a/doc/excel pruebas/ventas_2.xlsx
+++ b/doc/excel pruebas/ventas_2.xlsx
@@ -557,7 +557,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -567,8 +567,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:W11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="U10" sqref="U10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
@@ -750,7 +750,7 @@
       <c r="J3" t="s">
         <v>24</v>
       </c>
-      <c r="K3" s="6">
+      <c r="K3" s="5">
         <v>85600</v>
       </c>
       <c r="L3">
@@ -821,7 +821,7 @@
       <c r="J4" t="s">
         <v>24</v>
       </c>
-      <c r="K4" s="6">
+      <c r="K4" s="5">
         <v>2450000</v>
       </c>
       <c r="L4">
@@ -889,7 +889,7 @@
       <c r="J5" t="s">
         <v>44</v>
       </c>
-      <c r="K5" s="6">
+      <c r="K5" s="5">
         <v>3500</v>
       </c>
       <c r="L5">
@@ -960,7 +960,7 @@
       <c r="J6" t="s">
         <v>24</v>
       </c>
-      <c r="K6" s="6">
+      <c r="K6" s="5">
         <v>158300</v>
       </c>
       <c r="L6">
@@ -1028,7 +1028,7 @@
       <c r="J7" t="s">
         <v>24</v>
       </c>
-      <c r="K7" s="6">
+      <c r="K7" s="5">
         <v>94200</v>
       </c>
       <c r="L7">
@@ -1099,7 +1099,7 @@
       <c r="J8" t="s">
         <v>24</v>
       </c>
-      <c r="K8" s="6">
+      <c r="K8" s="5">
         <v>612000</v>
       </c>
       <c r="L8">
@@ -1167,7 +1167,7 @@
       <c r="J9" t="s">
         <v>24</v>
       </c>
-      <c r="K9" s="6">
+      <c r="K9" s="5">
         <v>42150</v>
       </c>
       <c r="L9">
@@ -1238,7 +1238,7 @@
       <c r="J10" t="s">
         <v>24</v>
       </c>
-      <c r="K10" s="6">
+      <c r="K10" s="5">
         <v>188900</v>
       </c>
       <c r="L10">
@@ -1306,7 +1306,7 @@
       <c r="J11" t="s">
         <v>24</v>
       </c>
-      <c r="K11" s="6">
+      <c r="K11" s="5">
         <v>75000</v>
       </c>
       <c r="L11">
@@ -1348,5 +1348,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>